<commit_message>
Tela de Login e MVC
</commit_message>
<xml_diff>
--- a/Sprint 7/Sprint_7 Burndown-Backlog.xlsx
+++ b/Sprint 7/Sprint_7 Burndown-Backlog.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="70">
   <si>
     <t>SPRINT BACKLOG</t>
   </si>
@@ -216,15 +216,6 @@
     <t>Mudanças de métodos das telas de agendamento para classse funcionário</t>
   </si>
   <si>
-    <t>Implementar métodos de consultas</t>
-  </si>
-  <si>
-    <t>Implementar parte gráfica da tela consulta</t>
-  </si>
-  <si>
-    <t>Exibir consultas do data atual na tela</t>
-  </si>
-  <si>
     <t>Não feito</t>
   </si>
   <si>
@@ -242,6 +233,21 @@
   <si>
     <t>Integração com agendamento</t>
   </si>
+  <si>
+    <t>Criação do banco, tabelas e atributos do banco</t>
+  </si>
+  <si>
+    <t>Implementar parte gráfica da tela consulta de agendamentos</t>
+  </si>
+  <si>
+    <t>Implementar métodos de consultas de agendamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exibir consultas do data atual na tela </t>
+  </si>
+  <si>
+    <t>Feito</t>
+  </si>
 </sst>
 </file>
 
@@ -251,7 +257,7 @@
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
     <numFmt numFmtId="165" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -358,6 +364,13 @@
     <font>
       <u/>
       <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
       <name val="Cambria"/>
       <family val="1"/>
       <charset val="1"/>
@@ -669,23 +682,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -696,8 +709,14 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -711,16 +730,16 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -756,14 +775,8 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2749,28 +2762,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.6875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.0625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.4375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -2882,31 +2895,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2934,11 +2947,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="187593920"/>
-        <c:axId val="188399856"/>
+        <c:axId val="190202040"/>
+        <c:axId val="190237144"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="187593920"/>
+        <c:axId val="190202040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3019,7 +3032,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188399856"/>
+        <c:crossAx val="190237144"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3027,7 +3040,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188399856"/>
+        <c:axId val="190237144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3078,7 +3091,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3110,7 +3122,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187593920"/>
+        <c:crossAx val="190202040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3123,7 +3135,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3260,28 +3271,28 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.6875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>4.875</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>4.0625</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>3.25</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2.4375</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1.625</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>0.8125</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0</c:v>
@@ -3393,31 +3404,31 @@
                 <c:formatCode>#,##0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>6.5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3445,11 +3456,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="187694384"/>
-        <c:axId val="187776104"/>
+        <c:axId val="190351024"/>
+        <c:axId val="191291880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="187694384"/>
+        <c:axId val="190351024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3491,7 +3502,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3523,7 +3533,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187776104"/>
+        <c:crossAx val="191291880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3531,7 +3541,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="187776104"/>
+        <c:axId val="191291880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3582,7 +3592,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -3614,7 +3623,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187694384"/>
+        <c:crossAx val="190351024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3627,7 +3636,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3949,11 +3957,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="187659352"/>
-        <c:axId val="188536632"/>
+        <c:axId val="191667480"/>
+        <c:axId val="191623432"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="187659352"/>
+        <c:axId val="191667480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3995,7 +4003,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4027,7 +4034,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188536632"/>
+        <c:crossAx val="191623432"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4035,7 +4042,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188536632"/>
+        <c:axId val="191623432"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4086,7 +4093,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4118,7 +4124,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="187659352"/>
+        <c:crossAx val="191667480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4131,7 +4137,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4453,11 +4458,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:smooth val="0"/>
-        <c:axId val="188543496"/>
-        <c:axId val="188544904"/>
+        <c:axId val="190929976"/>
+        <c:axId val="191635000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="188543496"/>
+        <c:axId val="190929976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4499,7 +4504,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4531,7 +4535,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188544904"/>
+        <c:crossAx val="191635000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4539,7 +4543,7 @@
         <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="188544904"/>
+        <c:axId val="191635000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4590,7 +4594,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -4622,7 +4625,7 @@
             <a:endParaRPr lang="pt-BR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="188543496"/>
+        <c:crossAx val="190929976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4635,7 +4638,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5102,10 +5104,10 @@
   <sheetPr>
     <tabColor rgb="FF38761D"/>
   </sheetPr>
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AB34"/>
   <sheetViews>
-    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView windowProtection="1" showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5122,16 +5124,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
       <c r="I1" s="2" t="s">
         <v>1</v>
       </c>
@@ -5156,27 +5158,27 @@
       <c r="AB1" s="4"/>
     </row>
     <row r="2" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A2" s="33" t="s">
+      <c r="A2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="33" t="s">
+      <c r="C2" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="33" t="s">
+      <c r="D2" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33" t="s">
+      <c r="E2" s="35"/>
+      <c r="F2" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="35"/>
+      <c r="H2" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="33">
+      <c r="I2" s="35">
         <v>8</v>
       </c>
       <c r="J2" s="3"/>
@@ -5200,9 +5202,9 @@
       <c r="AB2" s="4"/>
     </row>
     <row r="3" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
@@ -5215,8 +5217,8 @@
       <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
@@ -5238,25 +5240,29 @@
       <c r="AB3" s="4"/>
     </row>
     <row r="4" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="42" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="25">
+        <v>1</v>
+      </c>
       <c r="E4" s="39">
         <f>SUM(D4:D6)</f>
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="39">
         <f>SUM(F4:F6)</f>
         <v>0</v>
       </c>
-      <c r="H4" s="64" t="s">
-        <v>62</v>
+      <c r="H4" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="I4" s="30"/>
       <c r="J4" s="32"/>
@@ -5280,17 +5286,21 @@
       <c r="AB4" s="4"/>
     </row>
     <row r="5" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A5" s="37"/>
+      <c r="A5" s="43"/>
       <c r="B5" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="C5" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="25">
+        <v>1</v>
+      </c>
       <c r="E5" s="40"/>
       <c r="F5" s="25"/>
       <c r="G5" s="40"/>
-      <c r="H5" s="64" t="s">
-        <v>62</v>
+      <c r="H5" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="I5" s="31"/>
       <c r="J5" s="3"/>
@@ -5314,17 +5324,21 @@
       <c r="AB5" s="4"/>
     </row>
     <row r="6" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A6" s="38"/>
+      <c r="A6" s="44"/>
       <c r="B6" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
+      <c r="C6" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.5</v>
+      </c>
       <c r="E6" s="41"/>
       <c r="F6" s="27"/>
       <c r="G6" s="41"/>
-      <c r="H6" s="64" t="s">
-        <v>62</v>
+      <c r="H6" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="I6" s="31"/>
       <c r="J6" s="3"/>
@@ -5348,11 +5362,11 @@
       <c r="AB6" s="4"/>
     </row>
     <row r="7" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="34" t="s">
+      <c r="A7" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="28"/>
@@ -5365,8 +5379,8 @@
         <f>SUM(F7:F11)</f>
         <v>0</v>
       </c>
-      <c r="H7" s="64" t="s">
-        <v>62</v>
+      <c r="H7" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
@@ -5388,17 +5402,17 @@
       <c r="AB7" s="4"/>
     </row>
     <row r="8" spans="1:28" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="42"/>
+      <c r="A8" s="37"/>
       <c r="B8" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="20"/>
       <c r="E8" s="40"/>
       <c r="F8" s="20"/>
       <c r="G8" s="40"/>
-      <c r="H8" s="64" t="s">
-        <v>62</v>
+      <c r="H8" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="4"/>
@@ -5420,17 +5434,17 @@
       <c r="AB8" s="4"/>
     </row>
     <row r="9" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A9" s="42"/>
+      <c r="A9" s="37"/>
       <c r="B9" s="23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C9" s="20"/>
       <c r="D9" s="20"/>
       <c r="E9" s="40"/>
       <c r="F9" s="20"/>
       <c r="G9" s="40"/>
-      <c r="H9" s="64" t="s">
-        <v>62</v>
+      <c r="H9" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I9" s="6"/>
       <c r="K9" s="4"/>
@@ -5453,17 +5467,17 @@
       <c r="AB9" s="4"/>
     </row>
     <row r="10" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A10" s="42"/>
+      <c r="A10" s="37"/>
       <c r="B10" s="24" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="20"/>
       <c r="E10" s="40"/>
       <c r="F10" s="20"/>
       <c r="G10" s="40"/>
-      <c r="H10" s="64" t="s">
-        <v>62</v>
+      <c r="H10" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I10" s="6"/>
       <c r="K10" s="4"/>
@@ -5486,17 +5500,17 @@
       <c r="AB10" s="4"/>
     </row>
     <row r="11" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="35"/>
+      <c r="A11" s="38"/>
       <c r="B11" s="23" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
       <c r="E11" s="41"/>
       <c r="F11" s="20"/>
       <c r="G11" s="41"/>
-      <c r="H11" s="64" t="s">
-        <v>62</v>
+      <c r="H11" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I11" s="6"/>
       <c r="K11" s="4"/>
@@ -5519,25 +5533,29 @@
       <c r="AB11" s="4"/>
     </row>
     <row r="12" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A12" s="34" t="s">
+      <c r="A12" s="36" t="s">
         <v>39</v>
       </c>
       <c r="B12" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
+      <c r="C12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="20">
+        <v>1</v>
+      </c>
       <c r="E12" s="39">
         <f>SUM(D12:D13)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="39">
         <f>SUM(F12:F13)</f>
         <v>0</v>
       </c>
-      <c r="H12" s="64" t="s">
-        <v>62</v>
+      <c r="H12" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="I12" s="6"/>
       <c r="K12" s="4"/>
@@ -5560,17 +5578,21 @@
       <c r="AB12" s="4"/>
     </row>
     <row r="13" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
+      <c r="A13" s="38"/>
       <c r="B13" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
+      <c r="C13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="20">
+        <v>3</v>
+      </c>
       <c r="E13" s="41"/>
       <c r="F13" s="20"/>
       <c r="G13" s="41"/>
-      <c r="H13" s="64" t="s">
-        <v>62</v>
+      <c r="H13" s="34" t="s">
+        <v>69</v>
       </c>
       <c r="I13" s="6"/>
       <c r="K13" s="4"/>
@@ -5593,25 +5615,25 @@
       <c r="AB13" s="4"/>
     </row>
     <row r="14" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A14" s="62" t="s">
+      <c r="A14" s="36" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="22" t="s">
-        <v>49</v>
+      <c r="B14" s="24" t="s">
+        <v>65</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="20"/>
       <c r="E14" s="39">
-        <f>SUM(D14:D18)</f>
+        <f>SUM(D14:D19)</f>
         <v>0</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="39">
-        <f>SUM(F14:F18)</f>
-        <v>0</v>
-      </c>
-      <c r="H14" s="64" t="s">
-        <v>62</v>
+        <f>SUM(F14:F19)</f>
+        <v>0</v>
+      </c>
+      <c r="H14" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I14" s="6"/>
       <c r="K14" s="4"/>
@@ -5634,17 +5656,17 @@
       <c r="AB14" s="4"/>
     </row>
     <row r="15" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="62"/>
+      <c r="A15" s="37"/>
       <c r="B15" s="22" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="20"/>
       <c r="E15" s="40"/>
       <c r="F15" s="20"/>
       <c r="G15" s="40"/>
-      <c r="H15" s="64" t="s">
-        <v>62</v>
+      <c r="H15" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I15" s="6"/>
       <c r="K15" s="4"/>
@@ -5667,17 +5689,17 @@
       <c r="AB15" s="4"/>
     </row>
     <row r="16" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A16" s="62"/>
+      <c r="A16" s="37"/>
       <c r="B16" s="22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
+      <c r="D16" s="64"/>
       <c r="E16" s="40"/>
       <c r="F16" s="20"/>
       <c r="G16" s="40"/>
-      <c r="H16" s="64" t="s">
-        <v>62</v>
+      <c r="H16" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I16" s="6"/>
       <c r="K16" s="4"/>
@@ -5700,17 +5722,17 @@
       <c r="AB16" s="4"/>
     </row>
     <row r="17" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A17" s="62"/>
+      <c r="A17" s="37"/>
       <c r="B17" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="20"/>
       <c r="E17" s="40"/>
       <c r="F17" s="20"/>
       <c r="G17" s="40"/>
-      <c r="H17" s="64" t="s">
-        <v>62</v>
+      <c r="H17" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I17" s="6"/>
       <c r="K17" s="4"/>
@@ -5733,17 +5755,17 @@
       <c r="AB17" s="4"/>
     </row>
     <row r="18" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A18" s="62"/>
+      <c r="A18" s="37"/>
       <c r="B18" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="20"/>
-      <c r="E18" s="41"/>
+      <c r="E18" s="40"/>
       <c r="F18" s="20"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="64" t="s">
-        <v>62</v>
+      <c r="G18" s="40"/>
+      <c r="H18" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I18" s="6"/>
       <c r="K18" s="4"/>
@@ -5766,25 +5788,17 @@
       <c r="AB18" s="4"/>
     </row>
     <row r="19" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A19" s="34" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="63" t="s">
-        <v>60</v>
+      <c r="A19" s="38"/>
+      <c r="B19" s="22" t="s">
+        <v>53</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="20"/>
-      <c r="E19" s="39">
-        <f>SUM(D19:D21)</f>
-        <v>0</v>
-      </c>
+      <c r="E19" s="41"/>
       <c r="F19" s="20"/>
-      <c r="G19" s="39">
-        <f>SUM(F19:F21)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="64" t="s">
-        <v>62</v>
+      <c r="G19" s="41"/>
+      <c r="H19" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I19" s="6"/>
       <c r="K19" s="4"/>
@@ -5807,17 +5821,25 @@
       <c r="AB19" s="4"/>
     </row>
     <row r="20" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A20" s="42"/>
-      <c r="B20" s="22" t="s">
-        <v>59</v>
+      <c r="A20" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="33" t="s">
+        <v>66</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="20"/>
-      <c r="E20" s="40"/>
+      <c r="E20" s="39">
+        <f>SUM(D20:D22)</f>
+        <v>0</v>
+      </c>
       <c r="F20" s="20"/>
-      <c r="G20" s="40"/>
-      <c r="H20" s="64" t="s">
-        <v>62</v>
+      <c r="G20" s="39">
+        <f>SUM(F20:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="H20" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I20" s="6"/>
       <c r="K20" s="4"/>
@@ -5840,17 +5862,17 @@
       <c r="AB20" s="4"/>
     </row>
     <row r="21" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A21" s="35"/>
+      <c r="A21" s="37"/>
       <c r="B21" s="22" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="20"/>
-      <c r="E21" s="41"/>
+      <c r="E21" s="40"/>
       <c r="F21" s="20"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="64" t="s">
-        <v>62</v>
+      <c r="G21" s="40"/>
+      <c r="H21" s="34" t="s">
+        <v>59</v>
       </c>
       <c r="I21" s="6"/>
       <c r="K21" s="4"/>
@@ -5873,15 +5895,19 @@
       <c r="AB21" s="4"/>
     </row>
     <row r="22" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="29"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
+      <c r="A22" s="38"/>
+      <c r="B22" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="20"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="I22" s="6"/>
       <c r="K22" s="4"/>
       <c r="L22" s="4"/>
       <c r="M22" s="4"/>
@@ -5892,6 +5918,14 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+      <c r="Y22" s="4"/>
+      <c r="Z22" s="4"/>
+      <c r="AA22" s="4"/>
+      <c r="AB22" s="4"/>
     </row>
     <row r="23" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="6"/>
@@ -5899,7 +5933,7 @@
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="G23" s="29"/>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
@@ -5956,7 +5990,7 @@
       <c r="S25" s="4"/>
       <c r="T25" s="4"/>
     </row>
-    <row r="26" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="6"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -5977,7 +6011,7 @@
       <c r="S26" s="4"/>
       <c r="T26" s="4"/>
     </row>
-    <row r="27" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:28" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="6"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -5999,6 +6033,7 @@
       <c r="T27" s="4"/>
     </row>
     <row r="28" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
@@ -6059,8 +6094,6 @@
       <c r="T30" s="4"/>
     </row>
     <row r="31" spans="1:28" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
@@ -6124,24 +6157,46 @@
       <c r="S33" s="4"/>
       <c r="T33" s="4"/>
     </row>
+    <row r="34" spans="1:20" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+      <c r="H34" s="4"/>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="4"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+      <c r="T34" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="G19:G21"/>
-    <mergeCell ref="G14:G18"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="G7:G11"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E14:E18"/>
+    <mergeCell ref="G14:G19"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="E20:E22"/>
     <mergeCell ref="I2:I3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A18"/>
     <mergeCell ref="E12:E13"/>
     <mergeCell ref="E7:E11"/>
     <mergeCell ref="E4:E6"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="E14:E19"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="G7:G11"/>
+    <mergeCell ref="G4:G6"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
@@ -6193,20 +6248,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -6265,19 +6320,19 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="51" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -6295,10 +6350,10 @@
       <c r="J3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -6310,18 +6365,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="50"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -6336,35 +6391,35 @@
       </c>
       <c r="B5" s="12">
         <f>SUM('Sprint Backlog'!D:D)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0</v>
+        <v>5.6875</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.875</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0625</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.625</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="1"/>
@@ -6372,11 +6427,11 @@
       </c>
       <c r="K5" s="13">
         <f>SUM(C5:J5)</f>
-        <v>0</v>
+        <v>22.75</v>
       </c>
       <c r="L5" s="13">
         <f>K5/A$3</f>
-        <v>0</v>
+        <v>2.84375</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -6392,47 +6447,47 @@
       </c>
       <c r="B6" s="12">
         <f>B5</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="C6" s="13">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -6470,18 +6525,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -6496,7 +6551,7 @@
       </c>
       <c r="B9" s="16">
         <f>B5/A3</f>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:K9" si="3">SUM(C10:C12)</f>
@@ -6552,7 +6607,7 @@
       </c>
       <c r="B10" s="18">
         <f>Diogo!B9</f>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="C10" s="13">
         <f>Diogo!C9</f>
@@ -7222,20 +7277,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -7294,19 +7349,19 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="51" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -7324,10 +7379,10 @@
       <c r="J3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -7339,18 +7394,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="50"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -7365,35 +7420,35 @@
       </c>
       <c r="B5" s="12">
         <f>SUMIF('Sprint Backlog'!C:C,"=Diogo",'Sprint Backlog'!D:D)</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="C5" s="13">
         <f t="shared" ref="C5:J5" si="1">B5-$B9</f>
-        <v>0</v>
+        <v>5.6875</v>
       </c>
       <c r="D5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.875</v>
       </c>
       <c r="E5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.0625</v>
       </c>
       <c r="F5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.25</v>
       </c>
       <c r="G5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.4375</v>
       </c>
       <c r="H5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1.625</v>
       </c>
       <c r="I5" s="13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="J5" s="13">
         <f t="shared" si="1"/>
@@ -7401,11 +7456,11 @@
       </c>
       <c r="K5" s="13">
         <f>SUM(C5:J5)</f>
-        <v>0</v>
+        <v>22.75</v>
       </c>
       <c r="L5" s="13">
         <f>K5/A$3</f>
-        <v>0</v>
+        <v>2.84375</v>
       </c>
       <c r="M5" s="7"/>
       <c r="N5" s="7"/>
@@ -7421,47 +7476,47 @@
       </c>
       <c r="B6" s="12">
         <f>B5</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="C6" s="13">
         <f t="shared" ref="C6:J6" si="2">B6-C9</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="D6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="E6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="F6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="G6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="H6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="I6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="J6" s="13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="K6" s="13">
         <f>SUM(C6:J6)</f>
-        <v>0</v>
+        <v>52</v>
       </c>
       <c r="L6" s="13">
         <f>K6/A$3</f>
-        <v>0</v>
+        <v>6.5</v>
       </c>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
@@ -7499,18 +7554,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -7525,7 +7580,7 @@
       </c>
       <c r="B9" s="16">
         <f>B5/A3</f>
-        <v>0</v>
+        <v>0.8125</v>
       </c>
       <c r="C9" s="16">
         <f t="shared" ref="C9:L9" si="3">SUM(C10:C12)</f>
@@ -7576,10 +7631,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -7613,18 +7668,18 @@
         <v>0</v>
       </c>
       <c r="M10" s="7"/>
-      <c r="N10" s="59"/>
-      <c r="O10" s="59"/>
+      <c r="N10" s="61"/>
+      <c r="O10" s="61"/>
       <c r="P10" s="7"/>
       <c r="Q10" s="7"/>
       <c r="R10" s="7"/>
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="61"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -7658,18 +7713,18 @@
         <v>0</v>
       </c>
       <c r="M11" s="7"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="56"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
       <c r="P11" s="7"/>
       <c r="Q11" s="7"/>
       <c r="R11" s="7"/>
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="54"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -7703,18 +7758,18 @@
         <v>0</v>
       </c>
       <c r="M12" s="7"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="56"/>
+      <c r="N12" s="58"/>
+      <c r="O12" s="58"/>
       <c r="P12" s="7"/>
       <c r="Q12" s="7"/>
       <c r="R12" s="7"/>
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -7749,8 +7804,8 @@
       </c>
     </row>
     <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
+      <c r="A14" s="53"/>
+      <c r="B14" s="54"/>
     </row>
     <row r="1048573" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1048574" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -7833,20 +7888,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -7905,19 +7960,19 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="51" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -7935,10 +7990,10 @@
       <c r="J3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -7950,18 +8005,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="50"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -8110,18 +8165,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -8187,10 +8242,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="23.85" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -8232,10 +8287,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="57" t="s">
+      <c r="A11" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="58"/>
+      <c r="B11" s="60"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -8277,10 +8332,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
+      <c r="A12" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -8322,10 +8377,10 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="53" t="s">
+      <c r="A13" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B13" s="54"/>
+      <c r="B13" s="56"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>
@@ -8360,10 +8415,10 @@
       </c>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A14" s="55" t="s">
+      <c r="A14" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="55"/>
+      <c r="B14" s="57"/>
       <c r="C14" s="13">
         <v>0</v>
       </c>
@@ -8408,6 +8463,7 @@
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C8:L8"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:L1"/>
     <mergeCell ref="A3:A4"/>
@@ -8422,7 +8478,6 @@
     <mergeCell ref="J3:J4"/>
     <mergeCell ref="K3:K4"/>
     <mergeCell ref="L3:L4"/>
-    <mergeCell ref="C8:L8"/>
   </mergeCells>
   <conditionalFormatting sqref="C15:L96 K10:L10">
     <cfRule type="expression" dxfId="24" priority="17">
@@ -8522,20 +8577,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44" t="s">
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
       <c r="O1" s="7"/>
@@ -8594,19 +8649,19 @@
       <c r="S2" s="7"/>
     </row>
     <row r="3" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="45">
+      <c r="A3" s="47">
         <v>8</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="48" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="E3" s="47" t="s">
+      <c r="E3" s="51" t="s">
         <v>42</v>
       </c>
       <c r="F3" s="49" t="s">
@@ -8624,10 +8679,10 @@
       <c r="J3" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="K3" s="46" t="s">
+      <c r="K3" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="46" t="s">
+      <c r="L3" s="48" t="s">
         <v>15</v>
       </c>
       <c r="M3" s="7"/>
@@ -8639,18 +8694,18 @@
       <c r="S3" s="7"/>
     </row>
     <row r="4" spans="1:19" ht="14.25" x14ac:dyDescent="0.2">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
+      <c r="A4" s="47"/>
+      <c r="B4" s="48"/>
       <c r="C4" s="50"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="48"/>
+      <c r="D4" s="52"/>
+      <c r="E4" s="52"/>
       <c r="F4" s="50"/>
       <c r="G4" s="50"/>
       <c r="H4" s="50"/>
       <c r="I4" s="50"/>
       <c r="J4" s="50"/>
-      <c r="K4" s="46"/>
-      <c r="L4" s="46"/>
+      <c r="K4" s="48"/>
+      <c r="L4" s="48"/>
       <c r="M4" s="7"/>
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
@@ -8799,18 +8854,18 @@
       <c r="B8" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="43" t="s">
+      <c r="C8" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="43"/>
-      <c r="E8" s="43"/>
-      <c r="F8" s="43"/>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
-      <c r="K8" s="43"/>
-      <c r="L8" s="43"/>
+      <c r="D8" s="45"/>
+      <c r="E8" s="45"/>
+      <c r="F8" s="45"/>
+      <c r="G8" s="45"/>
+      <c r="H8" s="45"/>
+      <c r="I8" s="45"/>
+      <c r="J8" s="45"/>
+      <c r="K8" s="45"/>
+      <c r="L8" s="45"/>
       <c r="M8" s="7"/>
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
@@ -8876,10 +8931,10 @@
       <c r="S9" s="7"/>
     </row>
     <row r="10" spans="1:19" ht="21.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="58"/>
+      <c r="B10" s="60"/>
       <c r="C10" s="13">
         <v>0</v>
       </c>
@@ -8921,10 +8976,10 @@
       <c r="S10" s="7"/>
     </row>
     <row r="11" spans="1:19" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="61"/>
+      <c r="B11" s="63"/>
       <c r="C11" s="13">
         <v>0</v>
       </c>
@@ -8966,10 +9021,10 @@
       <c r="S11" s="7"/>
     </row>
     <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="53" t="s">
+      <c r="A12" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="54"/>
+      <c r="B12" s="56"/>
       <c r="C12" s="13">
         <v>0</v>
       </c>
@@ -9011,10 +9066,10 @@
       <c r="S12" s="7"/>
     </row>
     <row r="13" spans="1:19" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="55" t="s">
+      <c r="A13" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="55"/>
+      <c r="B13" s="57"/>
       <c r="C13" s="13">
         <v>0</v>
       </c>

</xml_diff>